<commit_message>
contact, proposal, FL updated
</commit_message>
<xml_diff>
--- a/Socheton/Contact/Contact_List.xlsx
+++ b/Socheton/Contact/Contact_List.xlsx
@@ -3,23 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CE7D5F-C315-4145-A8C8-777B6AFAF653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422C24EE-858C-4467-AAE9-C691E6BE1DC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SHED" sheetId="1" r:id="rId1"/>
     <sheet name="TMED" sheetId="3" r:id="rId2"/>
-    <sheet name="TECHEDU" sheetId="4" r:id="rId3"/>
-    <sheet name="MoEWOE" sheetId="5" r:id="rId4"/>
-    <sheet name="BMET" sheetId="6" r:id="rId5"/>
-    <sheet name="DYD" sheetId="7" r:id="rId6"/>
-    <sheet name="SEIP" sheetId="8" r:id="rId7"/>
-    <sheet name="ICTD" sheetId="9" r:id="rId8"/>
-    <sheet name="NGOAB" sheetId="10" r:id="rId9"/>
-    <sheet name="UN Entities BD" sheetId="11" r:id="rId10"/>
-    <sheet name="SMEF" sheetId="16" r:id="rId11"/>
-    <sheet name="BNFE" sheetId="17" r:id="rId12"/>
+    <sheet name="DME" sheetId="18" r:id="rId3"/>
+    <sheet name="TECHEDU" sheetId="4" r:id="rId4"/>
+    <sheet name="MoEWOE" sheetId="5" r:id="rId5"/>
+    <sheet name="BMET" sheetId="6" r:id="rId6"/>
+    <sheet name="DYD" sheetId="7" r:id="rId7"/>
+    <sheet name="SEIP" sheetId="8" r:id="rId8"/>
+    <sheet name="ICTD" sheetId="9" r:id="rId9"/>
+    <sheet name="NGOAB" sheetId="10" r:id="rId10"/>
+    <sheet name="UN Entities BD" sheetId="11" r:id="rId11"/>
+    <sheet name="SMEF" sheetId="16" r:id="rId12"/>
+    <sheet name="BNFE" sheetId="17" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2662" uniqueCount="1825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="1870">
   <si>
     <t>Name</t>
   </si>
@@ -5510,6 +5511,141 @@
   </si>
   <si>
     <t>Md. Wahiduzzaman</t>
+  </si>
+  <si>
+    <t>Directorate of Madrasha Education</t>
+  </si>
+  <si>
+    <t>Shafiuddin Ahmed</t>
+  </si>
+  <si>
+    <t>dg@dme.gov.bd</t>
+  </si>
+  <si>
+    <t>Md. Ziaul Ahsan</t>
+  </si>
+  <si>
+    <t>DIRECTOR (ADMIN &amp; FINANCE)</t>
+  </si>
+  <si>
+    <t>ziaulahsan0000@gmail.com</t>
+  </si>
+  <si>
+    <t>MOHAMMED SAJEDUL ISLAM</t>
+  </si>
+  <si>
+    <t>DIRECTOR (training &amp; development)</t>
+  </si>
+  <si>
+    <t>02-41030161</t>
+  </si>
+  <si>
+    <t>MD. SAIFUL ISLAM</t>
+  </si>
+  <si>
+    <t>DEPUTY DIRECTOR (ADMIN)</t>
+  </si>
+  <si>
+    <t>ddadmeb@gmail.com</t>
+  </si>
+  <si>
+    <t>Mohammad Samsuzzaman</t>
+  </si>
+  <si>
+    <t>DEPUTY DIRECTOR (FINANCE)</t>
+  </si>
+  <si>
+    <t>ddfinancedme@gmail.com</t>
+  </si>
+  <si>
+    <t>MOHAMMAD JAHANGIR ALAM</t>
+  </si>
+  <si>
+    <t>DEPUTY DIRECTOR (TRAINING &amp; DEVELOPMENT)</t>
+  </si>
+  <si>
+    <t>ddtraining.dme@gmail.com</t>
+  </si>
+  <si>
+    <t>MD. AFAZ UDDIN</t>
+  </si>
+  <si>
+    <t>ASSISTANT DIRECTOR (GOVT: &amp; SENIOR MADRASAH)</t>
+  </si>
+  <si>
+    <t>adsm.dme@gmail.com</t>
+  </si>
+  <si>
+    <t>ASSISTANT DIRECTOR (DAKHIL &amp; EBTEDIEE)</t>
+  </si>
+  <si>
+    <t>addakhil.dme@gmail.com</t>
+  </si>
+  <si>
+    <t>dmefarid@gamil.com</t>
+  </si>
+  <si>
+    <t>01751-560992</t>
+  </si>
+  <si>
+    <t>MD. ABDUL MUKIT</t>
+  </si>
+  <si>
+    <t>ASSISTANT DIRECTOR (LAW &amp; AUDIT)</t>
+  </si>
+  <si>
+    <t>adfinance.dme@gmail.com</t>
+  </si>
+  <si>
+    <t>addme.bd71@gamil.com</t>
+  </si>
+  <si>
+    <t>Inspector</t>
+  </si>
+  <si>
+    <t>inspectorkhulna.dme@gmail.com</t>
+  </si>
+  <si>
+    <t>badshaprog3@gmail.com</t>
+  </si>
+  <si>
+    <t>ferdousialam72@gmail.com</t>
+  </si>
+  <si>
+    <t>hossain_ict89@yahoo.com</t>
+  </si>
+  <si>
+    <t>emonamir1968@yahoo.com</t>
+  </si>
+  <si>
+    <t>Mahfuza Yeasmin</t>
+  </si>
+  <si>
+    <t>Md. Farid Ahmed</t>
+  </si>
+  <si>
+    <t>Assistant Director (Audir &amp; Law)</t>
+  </si>
+  <si>
+    <t>Md. Shahinur Islam</t>
+  </si>
+  <si>
+    <t>Md. Helal Uddin</t>
+  </si>
+  <si>
+    <t>Md. Badsha Mia</t>
+  </si>
+  <si>
+    <t>Mst. Ferdoushi Alam</t>
+  </si>
+  <si>
+    <t>Muhammad Hossain</t>
+  </si>
+  <si>
+    <t>Emon Amir</t>
+  </si>
+  <si>
+    <t>Information and Communication Technology Division</t>
   </si>
 </sst>
 </file>
@@ -5708,18 +5844,6 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5728,6 +5852,18 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6029,14 +6165,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
@@ -6289,7 +6425,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -6309,7 +6445,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -6329,7 +6465,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -6349,7 +6485,7 @@
         <v>1778380051</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -6369,7 +6505,7 @@
         <v>1713581397</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -6389,7 +6525,7 @@
         <v>1552343974</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -6409,7 +6545,7 @@
         <v>1676769036</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -6429,7 +6565,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -6449,7 +6585,7 @@
         <v>1731061760</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -6489,7 +6625,7 @@
         <v>1716505871</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -6549,7 +6685,7 @@
         <v>1715784765</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="28" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -6569,7 +6705,7 @@
         <v>1711353174</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -6589,7 +6725,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -6609,7 +6745,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -6629,7 +6765,7 @@
         <v>1912553070</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="32" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -6647,7 +6783,7 @@
       </c>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="33" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -6664,7 +6800,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="34" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -6701,7 +6837,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="36" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -6775,7 +6911,7 @@
         <v>1711015707</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="40" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -6795,7 +6931,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="41" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -6812,7 +6948,7 @@
         <v>1710052965</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="42" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -6832,7 +6968,7 @@
         <v>1764611292</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -6852,7 +6988,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="44" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -6872,7 +7008,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="45" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -6892,7 +7028,7 @@
         <v>1798596290</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="46" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -6912,7 +7048,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="47" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -6992,7 +7128,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="51" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -7012,7 +7148,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="52" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -7032,7 +7168,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="53" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A53" s="2">
         <v>51</v>
       </c>
@@ -7052,7 +7188,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="54" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -7072,7 +7208,7 @@
         <v>1732255144</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="55" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -7092,7 +7228,7 @@
         <v>1726224802</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="56" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -7112,7 +7248,7 @@
         <v>1552373357</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="57" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -7130,7 +7266,7 @@
       </c>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="58" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -7150,7 +7286,7 @@
         <v>1711904468</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="2" customFormat="1" ht="45">
+    <row r="59" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -7186,7 +7322,7 @@
       <c r="E60" s="18" t="s">
         <v>1636</v>
       </c>
-      <c r="F60" s="25">
+      <c r="F60" s="21">
         <v>29669813</v>
       </c>
     </row>
@@ -7390,6 +7526,534 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0566EEEB-7C01-455D-9C56-2211B8522E7E}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5">
+      <c r="A1" s="25" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>1482</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="17">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="17">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>774</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>1487</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>1488</v>
+      </c>
+      <c r="F4" s="19">
+        <v>1552380993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30">
+      <c r="A5" s="17">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F5" s="19">
+        <v>255007403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="17">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>1493</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>1494</v>
+      </c>
+      <c r="F6" s="19">
+        <v>255007404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" s="17">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>1497</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="17">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>1501</v>
+      </c>
+      <c r="F8" s="19">
+        <v>255007399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="17">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>1503</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>1504</v>
+      </c>
+      <c r="F9" s="19">
+        <v>255007394</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="17">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>1506</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>1507</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="17">
+        <v>9</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>1511</v>
+      </c>
+      <c r="F11" s="19">
+        <v>1531722984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="17">
+        <v>10</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>1511</v>
+      </c>
+      <c r="F12" s="19">
+        <v>255007395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="17">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F13" s="19">
+        <v>1729097455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="17">
+        <v>12</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>1518</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>1520</v>
+      </c>
+      <c r="F14" s="19">
+        <v>1911924252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="17">
+        <v>13</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F15" s="19">
+        <v>1718533373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{FCB98059-5141-49B2-94C7-BFC2AB84B572}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{8BE7DE8A-99ED-4765-81CE-25F76CF3A772}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{BD04441D-AAA5-4365-AC22-75F13D0DD860}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{3D33BAEF-B3DB-42D7-BEC5-2DC1E3EC974F}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{BCB266CE-715C-4CA1-B7CF-5EC945453B6E}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{1A8D1A27-D4ED-450A-AB7F-3543C37837B3}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{88333453-AA54-45C5-98A2-57D3A9C317E4}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{3BF32177-301F-472F-A09F-B8C3369B1A6B}"/>
+    <hyperlink ref="E14" r:id="rId9" xr:uid="{08D66F44-FF8B-4EB5-872B-42F7B6838868}"/>
+    <hyperlink ref="E15" r:id="rId10" xr:uid="{C1C384C2-1EB7-46A7-9CEE-462B8F24DB20}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13511AC9-EDD9-434B-912C-BDA7C318888D}">
   <dimension ref="A1:F37"/>
   <sheetViews>
@@ -7407,14 +8071,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>1523</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="17" t="s">
@@ -8006,7 +8670,7 @@
       <c r="E33" s="18" t="s">
         <v>1623</v>
       </c>
-      <c r="F33" s="24">
+      <c r="F33" s="20">
         <v>1310273936</v>
       </c>
     </row>
@@ -8026,7 +8690,7 @@
       <c r="E34" s="18" t="s">
         <v>1625</v>
       </c>
-      <c r="F34" s="24">
+      <c r="F34" s="20">
         <v>1681523496</v>
       </c>
     </row>
@@ -8064,7 +8728,7 @@
       <c r="E36" s="18" t="s">
         <v>1633</v>
       </c>
-      <c r="F36" s="26"/>
+      <c r="F36" s="22"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="17">
@@ -8082,7 +8746,7 @@
       <c r="E37" s="18" t="s">
         <v>1638</v>
       </c>
-      <c r="F37" s="26">
+      <c r="F37" s="22">
         <v>28159001</v>
       </c>
     </row>
@@ -8133,12 +8797,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF19544-DBBC-4EE4-8CDE-FB2F731FFCCB}">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8152,14 +8816,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5">
-      <c r="A1" s="23" t="s">
-        <v>1483</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="A1" s="25" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="17" t="s">
@@ -8231,7 +8895,7 @@
       <c r="C5" s="17" t="s">
         <v>1647</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="23" t="s">
         <v>1660</v>
       </c>
       <c r="E5" s="18" t="s">
@@ -8251,7 +8915,7 @@
       <c r="C6" s="17" t="s">
         <v>1647</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="23" t="s">
         <v>1661</v>
       </c>
       <c r="E6" s="18" t="s">
@@ -8271,7 +8935,7 @@
       <c r="C7" s="17" t="s">
         <v>1647</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="23" t="s">
         <v>1662</v>
       </c>
       <c r="E7" s="18" t="s">
@@ -8291,7 +8955,7 @@
       <c r="C8" s="17" t="s">
         <v>1653</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="23" t="s">
         <v>1663</v>
       </c>
       <c r="E8" s="18" t="s">
@@ -8311,7 +8975,7 @@
       <c r="C9" s="17" t="s">
         <v>1653</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="23" t="s">
         <v>1664</v>
       </c>
       <c r="E9" s="17" t="s">
@@ -8351,7 +9015,7 @@
       <c r="C11" s="17" t="s">
         <v>1658</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="23" t="s">
         <v>1667</v>
       </c>
       <c r="E11" s="18" t="s">
@@ -8371,7 +9035,7 @@
       <c r="C12" s="17" t="s">
         <v>1658</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>1670</v>
       </c>
       <c r="E12" s="18" t="s">
@@ -8391,7 +9055,7 @@
       <c r="C13" s="17" t="s">
         <v>1658</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="23" t="s">
         <v>1673</v>
       </c>
       <c r="E13" s="18" t="s">
@@ -8471,7 +9135,7 @@
       <c r="C17" s="17" t="s">
         <v>1658</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="23" t="s">
         <v>1686</v>
       </c>
       <c r="E17" s="18" t="s">
@@ -8491,7 +9155,7 @@
       <c r="C18" s="17" t="s">
         <v>1658</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="23" t="s">
         <v>1689</v>
       </c>
       <c r="E18" s="17" t="s">
@@ -8961,7 +9625,7 @@
         <v>1520101314</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="45">
+    <row r="42" spans="1:6" ht="30">
       <c r="A42" s="17">
         <v>40</v>
       </c>
@@ -9031,7 +9695,7 @@
       <c r="C45" s="17" t="s">
         <v>1736</v>
       </c>
-      <c r="D45" s="27" t="s">
+      <c r="D45" s="23" t="s">
         <v>1758</v>
       </c>
       <c r="E45" s="18" t="s">
@@ -9051,7 +9715,7 @@
       <c r="C46" s="17" t="s">
         <v>1736</v>
       </c>
-      <c r="D46" s="27" t="s">
+      <c r="D46" s="23" t="s">
         <v>1761</v>
       </c>
       <c r="E46" s="18" t="s">
@@ -9071,7 +9735,7 @@
       <c r="C47" s="17" t="s">
         <v>1736</v>
       </c>
-      <c r="D47" s="27" t="s">
+      <c r="D47" s="23" t="s">
         <v>1764</v>
       </c>
       <c r="E47" s="18" t="s">
@@ -9091,7 +9755,7 @@
       <c r="C48" s="17" t="s">
         <v>1736</v>
       </c>
-      <c r="D48" s="27" t="s">
+      <c r="D48" s="23" t="s">
         <v>1767</v>
       </c>
       <c r="E48" s="18" t="s">
@@ -9111,7 +9775,7 @@
       <c r="C49" s="17" t="s">
         <v>1736</v>
       </c>
-      <c r="D49" s="27" t="s">
+      <c r="D49" s="23" t="s">
         <v>1770</v>
       </c>
       <c r="E49" s="18" t="s">
@@ -9215,12 +9879,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B350BBE0-6406-4223-97B9-EABBA0BC7373}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9232,14 +9896,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>1778</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7">
@@ -9572,7 +10236,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9587,14 +10251,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
@@ -10307,6 +10971,397 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662A2A83-B6E2-40A7-A23B-D8E628DEF110}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5">
+      <c r="A1" s="25" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="17">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>1827</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1552318035</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="17">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>1828</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>1829</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>1830</v>
+      </c>
+      <c r="F4" s="19">
+        <v>1711944725</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30">
+      <c r="A5" s="17">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>1832</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="19" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30">
+      <c r="A6" s="17">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F6" s="19">
+        <v>1718019490</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" s="17">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>1838</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>1839</v>
+      </c>
+      <c r="F7" s="19">
+        <v>1711056876</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45">
+      <c r="A8" s="17">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>1840</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>1842</v>
+      </c>
+      <c r="F8" s="19">
+        <v>1718096058</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45">
+      <c r="A9" s="17">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>1844</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>1845</v>
+      </c>
+      <c r="F9" s="19">
+        <v>1718658910</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="17">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>1846</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>1847</v>
+      </c>
+      <c r="F10" s="19">
+        <v>1711359097</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="17">
+        <v>9</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>1862</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>1848</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="17">
+        <v>10</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>1851</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>1852</v>
+      </c>
+      <c r="F12" s="19">
+        <v>1911916877</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="17">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>1810</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>1853</v>
+      </c>
+      <c r="F13" s="19">
+        <v>1751375556</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30">
+      <c r="A14" s="17">
+        <v>12</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>1864</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>1855</v>
+      </c>
+      <c r="F14" s="19">
+        <v>1721444351</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="17">
+        <v>13</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>1856</v>
+      </c>
+      <c r="F15" s="19">
+        <v>1718938209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="17">
+        <v>14</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>1857</v>
+      </c>
+      <c r="F16" s="19">
+        <v>1716182232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F17" s="19">
+        <v>1813685510</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="17">
+        <v>16</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>1868</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>1859</v>
+      </c>
+      <c r="F18" s="19">
+        <v>1712726812</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{BAA1B904-0037-47D4-BECF-61014945885A}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{B6565F54-6339-4851-95D4-406391D93CBE}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{3E86EE84-C047-462F-B3A0-391D396637BC}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{73A6117A-6CAC-47FC-A53C-20A39F2FAD9E}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{F40AB10B-E7CE-456B-A958-A5A5542DD50A}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{FC23B9AD-A786-4159-9988-F7F2301A8E73}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{DDC51C53-2684-44FD-ADF5-E30E92C80DCE}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{6247C2C9-5D9A-4FF3-AB75-E899C1D3C88E}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{969F6244-EEA8-454D-9206-2BB75031DD55}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{99F0C690-0A52-4169-BA6A-39F07AE556A8}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{E56A235E-8A7C-4E73-AFFC-7D91AE2C4C0C}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{B226D26C-5033-4654-A8EB-A79DDCCCEA2C}"/>
+    <hyperlink ref="E16" r:id="rId13" xr:uid="{BB1524AD-744C-4614-BB68-1680DA9D0946}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{47EAD319-ABB6-4514-AA59-1C45FC440884}"/>
+    <hyperlink ref="E18" r:id="rId15" xr:uid="{EA46E02B-D475-47F8-B93A-6C67F41F648A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E355C957-C9F2-4240-BF7D-3223C10FC84E}">
   <dimension ref="A1:F52"/>
   <sheetViews>
@@ -10324,14 +11379,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
@@ -10633,7 +11688,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="60">
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="45">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -11329,12 +12384,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9FE0DC-0546-4303-A31D-84FCDB11FAD1}">
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11347,14 +12402,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>412</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -12277,7 +13332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20679603-B946-4BC4-B9FE-5A6CB3B25D6C}">
   <dimension ref="A1:F89"/>
   <sheetViews>
@@ -12295,14 +13350,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -12364,7 +13419,7 @@
         <v>1936993651</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30">
+    <row r="5" spans="1:6" ht="45">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -14033,7 +15088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825B2715-03B3-43B9-B5A7-95117B70CB41}">
   <dimension ref="A1:F42"/>
   <sheetViews>
@@ -14051,14 +15106,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>739</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -14891,7 +15946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA97054-2957-4A5E-85E9-9ED43C6A2756}">
   <dimension ref="A1:F186"/>
   <sheetViews>
@@ -14909,14 +15964,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>873</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -16725,7 +17780,7 @@
       <c r="B92" s="8" t="s">
         <v>1153</v>
       </c>
-      <c r="C92" s="21" t="s">
+      <c r="C92" s="26" t="s">
         <v>1154</v>
       </c>
       <c r="D92" s="8" t="s">
@@ -16745,7 +17800,7 @@
       <c r="B93" s="8" t="s">
         <v>1156</v>
       </c>
-      <c r="C93" s="22"/>
+      <c r="C93" s="27"/>
       <c r="D93" s="8" t="s">
         <v>1175</v>
       </c>
@@ -18645,12 +19700,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D2DA89-2D91-4E66-BE4F-EE783D5328E7}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18665,14 +19720,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5">
-      <c r="A1" s="20" t="s">
-        <v>873</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="A1" s="24" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -19259,532 +20314,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0566EEEB-7C01-455D-9C56-2211B8522E7E}">
-  <dimension ref="A1:F40"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="25.5">
-      <c r="A1" s="23" t="s">
-        <v>1483</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>1482</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>1484</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>277</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>1485</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>1486</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30">
-      <c r="A4" s="17">
-        <v>2</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>774</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>1487</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>1488</v>
-      </c>
-      <c r="F4" s="19">
-        <v>1552380993</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30">
-      <c r="A5" s="17">
-        <v>3</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>1489</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>1490</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>1491</v>
-      </c>
-      <c r="F5" s="19">
-        <v>255007403</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="17">
-        <v>4</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>1493</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>1494</v>
-      </c>
-      <c r="F6" s="19">
-        <v>255007404</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30">
-      <c r="A7" s="17">
-        <v>5</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>1495</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>1496</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>1497</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>1498</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30">
-      <c r="A8" s="17">
-        <v>6</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>1499</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>1500</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>1501</v>
-      </c>
-      <c r="F8" s="19">
-        <v>255007399</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30">
-      <c r="A9" s="17">
-        <v>7</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>1502</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>1503</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>1504</v>
-      </c>
-      <c r="F9" s="19">
-        <v>255007394</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30">
-      <c r="A10" s="17">
-        <v>8</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>1505</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>1506</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>1507</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>1508</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30">
-      <c r="A11" s="17">
-        <v>9</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>1509</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>1510</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>1511</v>
-      </c>
-      <c r="F11" s="19">
-        <v>1531722984</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30">
-      <c r="A12" s="17">
-        <v>10</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>1512</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>1513</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>1511</v>
-      </c>
-      <c r="F12" s="19">
-        <v>255007395</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="17">
-        <v>11</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>1514</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>1515</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>1516</v>
-      </c>
-      <c r="F13" s="19">
-        <v>1729097455</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="17">
-        <v>12</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>1517</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>1518</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>1520</v>
-      </c>
-      <c r="F14" s="19">
-        <v>1911924252</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="17">
-        <v>13</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>1521</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>1519</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>1522</v>
-      </c>
-      <c r="F15" s="19">
-        <v>1718533373</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{FCB98059-5141-49B2-94C7-BFC2AB84B572}"/>
-    <hyperlink ref="E5" r:id="rId2" xr:uid="{8BE7DE8A-99ED-4765-81CE-25F76CF3A772}"/>
-    <hyperlink ref="E6" r:id="rId3" xr:uid="{BD04441D-AAA5-4365-AC22-75F13D0DD860}"/>
-    <hyperlink ref="E7" r:id="rId4" xr:uid="{3D33BAEF-B3DB-42D7-BEC5-2DC1E3EC974F}"/>
-    <hyperlink ref="E8" r:id="rId5" xr:uid="{BCB266CE-715C-4CA1-B7CF-5EC945453B6E}"/>
-    <hyperlink ref="E9" r:id="rId6" xr:uid="{1A8D1A27-D4ED-450A-AB7F-3543C37837B3}"/>
-    <hyperlink ref="E10" r:id="rId7" xr:uid="{88333453-AA54-45C5-98A2-57D3A9C317E4}"/>
-    <hyperlink ref="E13" r:id="rId8" xr:uid="{3BF32177-301F-472F-A09F-B8C3369B1A6B}"/>
-    <hyperlink ref="E14" r:id="rId9" xr:uid="{08D66F44-FF8B-4EB5-872B-42F7B6838868}"/>
-    <hyperlink ref="E15" r:id="rId10" xr:uid="{C1C384C2-1EB7-46A7-9CEE-462B8F24DB20}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
-</worksheet>
 </file>
</xml_diff>